<commit_message>
adding userstories and requirements to rtm example
</commit_message>
<xml_diff>
--- a/Project 1/Example-RTM.xlsx
+++ b/Project 1/Example-RTM.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricSuminski\Desktop\250704-JWA\Project 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E34C739-A1AD-461B-AC72-D3E895162165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A17EC8-8C9A-4D54-999F-2A093B9D3F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{786AC32F-343F-4356-AB12-C2F923337BD5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{786AC32F-343F-4356-AB12-C2F923337BD5}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
+    <sheet name="SRS" sheetId="2" r:id="rId2"/>
+    <sheet name="User Story Req. Mapping" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
   <si>
     <t>As a new user I want to open an account with the Planetarium so I can save my celestial findings</t>
   </si>
@@ -59,19 +61,175 @@
     <t>User Story ID</t>
   </si>
   <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>U5</t>
+    <t>Security Requirements</t>
+  </si>
+  <si>
+    <t>Security Requirements ID</t>
+  </si>
+  <si>
+    <t>Passwords should never be visible in plain text</t>
+  </si>
+  <si>
+    <t>Users should only be able to interact with resources they have added to the Planetarium</t>
+  </si>
+  <si>
+    <t>Only logged in Users should be able to access the Planetarium home page</t>
+  </si>
+  <si>
+    <t>User Requirements ID</t>
+  </si>
+  <si>
+    <t>User Requirement</t>
+  </si>
+  <si>
+    <t>Users should have unique usernames</t>
+  </si>
+  <si>
+    <t>Usernames and passwords should be between 5-30 characters</t>
+  </si>
+  <si>
+    <t>Usernames and passwords should start with a letter</t>
+  </si>
+  <si>
+    <t>Usernames should support lower case, upper case, numeric characters, underscores, and dashes</t>
+  </si>
+  <si>
+    <t>Passwords should contain a lower case, upper case, and numeric character</t>
+  </si>
+  <si>
+    <t>Passwords should support underscores and dashes</t>
+  </si>
+  <si>
+    <t>US1</t>
+  </si>
+  <si>
+    <t>US2</t>
+  </si>
+  <si>
+    <t>US3</t>
+  </si>
+  <si>
+    <t>US4</t>
+  </si>
+  <si>
+    <t>US5</t>
+  </si>
+  <si>
+    <t>SR1</t>
+  </si>
+  <si>
+    <t>SR2</t>
+  </si>
+  <si>
+    <t>SR3</t>
+  </si>
+  <si>
+    <t>UR1</t>
+  </si>
+  <si>
+    <t>UR2</t>
+  </si>
+  <si>
+    <t>UR3</t>
+  </si>
+  <si>
+    <t>UR4</t>
+  </si>
+  <si>
+    <t>UR5</t>
+  </si>
+  <si>
+    <t>UR6</t>
+  </si>
+  <si>
+    <t>Planet Requirements ID</t>
+  </si>
+  <si>
+    <t>Planet Requirement</t>
+  </si>
+  <si>
+    <t>Planet names should be between 1-30 characters</t>
+  </si>
+  <si>
+    <t>Planet names should support lower case, upper case, numeric characters, white space, underscores, and dashes</t>
+  </si>
+  <si>
+    <t>Planets should have unique names</t>
+  </si>
+  <si>
+    <t>Planets should be “owned” by the user that added it to the Planetarium</t>
+  </si>
+  <si>
+    <t>Planets should allow adding an associated image, but an image should not be required for the data to be added to the database</t>
+  </si>
+  <si>
+    <t>JPEG &amp; PNG should be supported</t>
+  </si>
+  <si>
+    <t>PR1</t>
+  </si>
+  <si>
+    <t>PR2</t>
+  </si>
+  <si>
+    <t>PR3</t>
+  </si>
+  <si>
+    <t>PR4</t>
+  </si>
+  <si>
+    <t>PR5</t>
+  </si>
+  <si>
+    <t>PR6</t>
+  </si>
+  <si>
+    <t>Moon Requirements ID</t>
+  </si>
+  <si>
+    <t>Moon Requirement</t>
+  </si>
+  <si>
+    <t>Moon names should be between 1-30 characters</t>
+  </si>
+  <si>
+    <t>Moon names should support lower case, upper case, numeric characters, white space, underscores, and dashes</t>
+  </si>
+  <si>
+    <t>Moons should have unique names</t>
+  </si>
+  <si>
+    <t>Moons should be “owned” by the Planet the User adding the moon associated it with</t>
+  </si>
+  <si>
+    <t>Moons should be deleted if their "owner" planet is deleted from the database</t>
+  </si>
+  <si>
+    <t>Moons should allow adding an associated image, but an image should not be required for the data to be added to the database</t>
+  </si>
+  <si>
+    <t>MR1</t>
+  </si>
+  <si>
+    <t>MR2</t>
+  </si>
+  <si>
+    <t>MR3</t>
+  </si>
+  <si>
+    <t>MR4</t>
+  </si>
+  <si>
+    <t>MR5</t>
+  </si>
+  <si>
+    <t>MR6</t>
+  </si>
+  <si>
+    <t>MR7</t>
+  </si>
+  <si>
+    <t>Requirement ID</t>
   </si>
 </sst>
 </file>
@@ -107,8 +265,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -119,7 +280,46 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="16">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -143,13 +343,57 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A1D89500-C288-4E85-931C-4E8E350EFE9F}" name="Table1" displayName="Table1" ref="A1:B6" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A1D89500-C288-4E85-931C-4E8E350EFE9F}" name="Table1" displayName="Table1" ref="A1:B6" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A1:B6" xr:uid="{A1D89500-C288-4E85-931C-4E8E350EFE9F}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{50438F80-F423-492F-8BAB-9BD01C0E6EBD}" name="User Story ID" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{37B1E00F-6EFE-429A-B889-34A77822F27E}" name="User Stories" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{50438F80-F423-492F-8BAB-9BD01C0E6EBD}" name="User Story ID" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{37B1E00F-6EFE-429A-B889-34A77822F27E}" name="User Stories" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{592C5268-2408-4D04-A18B-D290F2BF14BC}" name="Table2" displayName="Table2" ref="A1:B4" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:B4" xr:uid="{592C5268-2408-4D04-A18B-D290F2BF14BC}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{1F5F49C2-BA2D-46FF-B7C6-3CA1F3C4317D}" name="Security Requirements ID" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{14EF36D4-0F3F-424A-A991-CB4BEF02426F}" name="Security Requirements" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0D51DAC4-EC7E-4E56-A0AB-386CD380A8F2}" name="Table3" displayName="Table3" ref="C1:D7" totalsRowShown="0">
+  <autoFilter ref="C1:D7" xr:uid="{0D51DAC4-EC7E-4E56-A0AB-386CD380A8F2}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{B9849CD9-577F-4FF1-9FBE-415672003CCB}" name="User Requirements ID"/>
+    <tableColumn id="2" xr3:uid="{CEA8AAC1-E5CD-4885-B8C3-C984E7A332DA}" name="User Requirement" dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{70C9C6D4-BAAE-40EC-A7DF-32D56E7036E6}" name="Table4" displayName="Table4" ref="E1:F7" totalsRowShown="0" headerRowDxfId="4" dataDxfId="5">
+  <autoFilter ref="E1:F7" xr:uid="{70C9C6D4-BAAE-40EC-A7DF-32D56E7036E6}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{C9987381-35F5-4FBE-9273-54C79E5B0FDF}" name="Planet Requirements ID" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{0DC7E240-03EC-4B61-9B0E-3710A36AB6F2}" name="Planet Requirement" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F72E17BE-32D2-44BE-A323-3E19C635C91F}" name="Table5" displayName="Table5" ref="G1:H8" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="G1:H8" xr:uid="{F72E17BE-32D2-44BE-A323-3E19C635C91F}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{F17BD771-15DB-43F1-83DF-9CD3FF4C8E1E}" name="Moon Requirements ID" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{2587E061-851C-4E57-97E9-C28EA2F35AB8}" name="Moon Requirement" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -472,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3188B723-0C94-4D3B-9499-A9BB00207D84}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,50 +727,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -536,4 +780,234 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDED5571-6071-483B-91FF-46A3D4DE2E17}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" customWidth="1"/>
+    <col min="7" max="7" width="26" customWidth="1"/>
+    <col min="8" max="8" width="27.5703125" customWidth="1"/>
+    <col min="9" max="9" width="28.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="G8" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="4">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7F44907-20F8-4A20-B214-72FF20079D8A}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding US1 requirements mappings
</commit_message>
<xml_diff>
--- a/Project 1/Example-RTM.xlsx
+++ b/Project 1/Example-RTM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricSuminski\Desktop\250704-JWA\Project 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A17EC8-8C9A-4D54-999F-2A093B9D3F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863EBA65-D303-4326-9915-80B6FAE5CF91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{786AC32F-343F-4356-AB12-C2F923337BD5}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="64">
   <si>
     <t>As a new user I want to open an account with the Planetarium so I can save my celestial findings</t>
   </si>
@@ -394,6 +394,23 @@
     <tableColumn id="2" xr3:uid="{2587E061-851C-4E57-97E9-C28EA2F35AB8}" name="Moon Requirement" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5D6C84DD-1634-44D6-8697-8367F7D74DA9}" name="Table6" displayName="Table6" ref="A1:B10" totalsRowShown="0">
+  <autoFilter ref="A1:B10" xr:uid="{5D6C84DD-1634-44D6-8697-8367F7D74DA9}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="US1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{67C35128-8397-490E-8082-E2191E708F71}" name="User Story ID"/>
+    <tableColumn id="2" xr3:uid="{D714C834-C546-4113-8A2A-28987BB42645}" name="Requirement ID"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -717,7 +734,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,7 +804,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,11 +1005,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7F44907-20F8-4A20-B214-72FF20079D8A}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1007,7 +1022,79 @@
         <v>63</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding more general testing notes
</commit_message>
<xml_diff>
--- a/Project 1/Example-RTM.xlsx
+++ b/Project 1/Example-RTM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricSuminski\Desktop\250704-JWA\Project 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863EBA65-D303-4326-9915-80B6FAE5CF91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F122B28-C964-4DD6-BE76-9AC30F3EDA0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{786AC32F-343F-4356-AB12-C2F923337BD5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{786AC32F-343F-4356-AB12-C2F923337BD5}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
@@ -321,10 +321,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -343,11 +343,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A1D89500-C288-4E85-931C-4E8E350EFE9F}" name="Table1" displayName="Table1" ref="A1:B6" totalsRowShown="0" headerRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A1D89500-C288-4E85-931C-4E8E350EFE9F}" name="Table1" displayName="Table1" ref="A1:B6" totalsRowShown="0" headerRowDxfId="15">
   <autoFilter ref="A1:B6" xr:uid="{A1D89500-C288-4E85-931C-4E8E350EFE9F}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{50438F80-F423-492F-8BAB-9BD01C0E6EBD}" name="User Story ID" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{37B1E00F-6EFE-429A-B889-34A77822F27E}" name="User Stories" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{50438F80-F423-492F-8BAB-9BD01C0E6EBD}" name="User Story ID" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{37B1E00F-6EFE-429A-B889-34A77822F27E}" name="User Stories" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -376,22 +376,22 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{70C9C6D4-BAAE-40EC-A7DF-32D56E7036E6}" name="Table4" displayName="Table4" ref="E1:F7" totalsRowShown="0" headerRowDxfId="4" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{70C9C6D4-BAAE-40EC-A7DF-32D56E7036E6}" name="Table4" displayName="Table4" ref="E1:F7" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="E1:F7" xr:uid="{70C9C6D4-BAAE-40EC-A7DF-32D56E7036E6}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{C9987381-35F5-4FBE-9273-54C79E5B0FDF}" name="Planet Requirements ID" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{0DC7E240-03EC-4B61-9B0E-3710A36AB6F2}" name="Planet Requirement" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{C9987381-35F5-4FBE-9273-54C79E5B0FDF}" name="Planet Requirements ID" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{0DC7E240-03EC-4B61-9B0E-3710A36AB6F2}" name="Planet Requirement" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F72E17BE-32D2-44BE-A323-3E19C635C91F}" name="Table5" displayName="Table5" ref="G1:H8" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F72E17BE-32D2-44BE-A323-3E19C635C91F}" name="Table5" displayName="Table5" ref="G1:H8" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="G1:H8" xr:uid="{F72E17BE-32D2-44BE-A323-3E19C635C91F}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F17BD771-15DB-43F1-83DF-9CD3FF4C8E1E}" name="Moon Requirements ID" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{2587E061-851C-4E57-97E9-C28EA2F35AB8}" name="Moon Requirement" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{F17BD771-15DB-43F1-83DF-9CD3FF4C8E1E}" name="Moon Requirements ID" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{2587E061-851C-4E57-97E9-C28EA2F35AB8}" name="Moon Requirement" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -803,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDED5571-6071-483B-91FF-46A3D4DE2E17}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,7 +1007,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7F44907-20F8-4A20-B214-72FF20079D8A}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
adding more notes/examples for rtm
</commit_message>
<xml_diff>
--- a/Project 1/Example-RTM.xlsx
+++ b/Project 1/Example-RTM.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricSuminski\Desktop\250704-JWA\Project 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F122B28-C964-4DD6-BE76-9AC30F3EDA0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DDCB3A3-9926-41E3-90D5-27104BCE0605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{786AC32F-343F-4356-AB12-C2F923337BD5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{786AC32F-343F-4356-AB12-C2F923337BD5}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
     <sheet name="SRS" sheetId="2" r:id="rId2"/>
     <sheet name="User Story Req. Mapping" sheetId="3" r:id="rId3"/>
+    <sheet name="AC" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="72">
   <si>
     <t>As a new user I want to open an account with the Planetarium so I can save my celestial findings</t>
   </si>
@@ -230,6 +231,30 @@
   </si>
   <si>
     <t>Requirement ID</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>Happy Path</t>
+  </si>
+  <si>
+    <t>Given the user is on the login page</t>
+  </si>
+  <si>
+    <t>When the user clicks the register link</t>
+  </si>
+  <si>
+    <t>When the user provides a valid username</t>
+  </si>
+  <si>
+    <t>And the user provides a valid password</t>
+  </si>
+  <si>
+    <t>Then an alert should appear saying "Account created succssefully"</t>
+  </si>
+  <si>
+    <t>And the user should be redirected to the login page</t>
   </si>
 </sst>
 </file>
@@ -265,13 +290,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -734,7 +765,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDED5571-6071-483B-91FF-46A3D4DE2E17}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,7 +1039,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1099,4 +1130,66 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EECB696-23F9-45C5-BCAE-323A57C84042}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="36.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="5"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding testing pyramid notes
</commit_message>
<xml_diff>
--- a/Project 1/Example-RTM.xlsx
+++ b/Project 1/Example-RTM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricSuminski\Desktop\250704-JWA\Project 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DDCB3A3-9926-41E3-90D5-27104BCE0605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27053C33-E857-4BB6-862F-D59D1BDF7B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{786AC32F-343F-4356-AB12-C2F923337BD5}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="78">
   <si>
     <t>As a new user I want to open an account with the Planetarium so I can save my celestial findings</t>
   </si>
@@ -255,6 +255,24 @@
   </si>
   <si>
     <t>And the user should be redirected to the login page</t>
+  </si>
+  <si>
+    <t>Sad Path</t>
+  </si>
+  <si>
+    <t>And the user provides invalid credential data</t>
+  </si>
+  <si>
+    <t>Then the user should be shown an alert with an error message</t>
+  </si>
+  <si>
+    <t>And the user should remain on the register page</t>
+  </si>
+  <si>
+    <t>*Note*: This broader form of acceptance criteria is fine, just keep in mind for your actual tests you will need to break it down into more atomic steps</t>
+  </si>
+  <si>
+    <t>*Note*: this style of specific acceptance criteria is closer to what you will use for your tests, but for some user stories being specific with your AC will require creating multiple groupings of AC, which can be time consuming</t>
   </si>
 </sst>
 </file>
@@ -270,12 +288,42 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -290,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -301,11 +349,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -765,7 +822,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,7 +892,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1134,10 +1191,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EECB696-23F9-45C5-BCAE-323A57C84042}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1146,45 +1203,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>65</v>
       </c>
+      <c r="B2" s="7" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>66</v>
       </c>
+      <c r="B3" s="8" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>67</v>
       </c>
+      <c r="B4" s="8" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="B5" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>69</v>
       </c>
+      <c r="B6" s="8" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="B7" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>71</v>
       </c>
+      <c r="B8" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
adding notes about test data creation
</commit_message>
<xml_diff>
--- a/Project 1/Example-RTM.xlsx
+++ b/Project 1/Example-RTM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricSuminski\Desktop\250704-JWA\Project 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27053C33-E857-4BB6-862F-D59D1BDF7B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6733C5FD-1672-4031-9187-0E164C37797D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{786AC32F-343F-4356-AB12-C2F923337BD5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{786AC32F-343F-4356-AB12-C2F923337BD5}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
@@ -891,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDED5571-6071-483B-91FF-46A3D4DE2E17}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,7 +1193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EECB696-23F9-45C5-BCAE-323A57C84042}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adding example test data to rtm
</commit_message>
<xml_diff>
--- a/Project 1/Example-RTM.xlsx
+++ b/Project 1/Example-RTM.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricSuminski\Desktop\250704-JWA\Project 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6733C5FD-1672-4031-9187-0E164C37797D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD3A88E-337C-40D3-83E2-00144980C107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{786AC32F-343F-4356-AB12-C2F923337BD5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{786AC32F-343F-4356-AB12-C2F923337BD5}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
     <sheet name="SRS" sheetId="2" r:id="rId2"/>
     <sheet name="User Story Req. Mapping" sheetId="3" r:id="rId3"/>
     <sheet name="AC" sheetId="4" r:id="rId4"/>
+    <sheet name="Test Data" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="123">
   <si>
     <t>As a new user I want to open an account with the Planetarium so I can save my celestial findings</t>
   </si>
@@ -273,13 +274,148 @@
   </si>
   <si>
     <t>*Note*: this style of specific acceptance criteria is closer to what you will use for your tests, but for some user stories being specific with your AC will require creating multiple groupings of AC, which can be time consuming</t>
+  </si>
+  <si>
+    <t>Robin</t>
+  </si>
+  <si>
+    <t>bobby</t>
+  </si>
+  <si>
+    <t>thisshouldbethirtycharactersss</t>
+  </si>
+  <si>
+    <t>Unique Username &amp; start with letter</t>
+  </si>
+  <si>
+    <t>5 characters &amp; start with letter</t>
+  </si>
+  <si>
+    <t>30 characters &amp; start with letter</t>
+  </si>
+  <si>
+    <t>Robin_1-5</t>
+  </si>
+  <si>
+    <t>supports upper, lower numeric, dash, underscore</t>
+  </si>
+  <si>
+    <t>Non unique username</t>
+  </si>
+  <si>
+    <t>Batman</t>
+  </si>
+  <si>
+    <t>4 characters</t>
+  </si>
+  <si>
+    <t>31 characters</t>
+  </si>
+  <si>
+    <t>bobb</t>
+  </si>
+  <si>
+    <t>thisoverthirtycharacterssssssss</t>
+  </si>
+  <si>
+    <t>includes unsupported characters</t>
+  </si>
+  <si>
+    <t>**NOTE: Security Requirements will not require formal test data, since validating they are enforced is going to be a bit different from the other requirements</t>
+  </si>
+  <si>
+    <t>Robin!%?</t>
+  </si>
+  <si>
+    <t>Valid Username Test Data</t>
+  </si>
+  <si>
+    <t>Invalid Username Test Data</t>
+  </si>
+  <si>
+    <t>Valid Password Test Data</t>
+  </si>
+  <si>
+    <t>5 characters with required characters</t>
+  </si>
+  <si>
+    <t>30 characters with required characters</t>
+  </si>
+  <si>
+    <t>Bobb1</t>
+  </si>
+  <si>
+    <t>Thisshouldbethirtycharacterss3</t>
+  </si>
+  <si>
+    <t>supports dashes and underscores</t>
+  </si>
+  <si>
+    <t>Bob_b-1</t>
+  </si>
+  <si>
+    <t>Invalid Password Test Data</t>
+  </si>
+  <si>
+    <t>4 character password</t>
+  </si>
+  <si>
+    <t>31 character password</t>
+  </si>
+  <si>
+    <t>Bob3</t>
+  </si>
+  <si>
+    <t>Thisoverthirtycharactersssssss3</t>
+  </si>
+  <si>
+    <t>Username not starting with letter</t>
+  </si>
+  <si>
+    <t>3obin</t>
+  </si>
+  <si>
+    <t>not all required characters present</t>
+  </si>
+  <si>
+    <t>Bobby</t>
+  </si>
+  <si>
+    <t>bobb3</t>
+  </si>
+  <si>
+    <t>BOBB3</t>
+  </si>
+  <si>
+    <t>unsupported characters</t>
+  </si>
+  <si>
+    <t>Bobb3!?</t>
+  </si>
+  <si>
+    <t>Requirment ID</t>
+  </si>
+  <si>
+    <t>UR1, UR3</t>
+  </si>
+  <si>
+    <t>UR2, UR3, UR5</t>
+  </si>
+  <si>
+    <t>non-letter character at start</t>
+  </si>
+  <si>
+    <t>3obbY</t>
+  </si>
+  <si>
+    <t>**NOTE**: the goal of organizing your test data in this way is to make sure that you are covering all associated requirements with your test data. As long as all requirements have associated valid and invalid test data, you can be confident that your tests will sufficiently validate the user stories adhere to their related requirements</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,8 +423,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -325,6 +468,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -338,7 +499,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -355,14 +516,33 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -442,8 +622,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{592C5268-2408-4D04-A18B-D290F2BF14BC}" name="Table2" displayName="Table2" ref="A1:B4" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:B4" xr:uid="{592C5268-2408-4D04-A18B-D290F2BF14BC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{592C5268-2408-4D04-A18B-D290F2BF14BC}" name="Table2" displayName="Table2" ref="A1:B5" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:B5" xr:uid="{592C5268-2408-4D04-A18B-D290F2BF14BC}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{1F5F49C2-BA2D-46FF-B7C6-3CA1F3C4317D}" name="Security Requirements ID" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{14EF36D4-0F3F-424A-A991-CB4BEF02426F}" name="Security Requirements" dataDxfId="9"/>
@@ -821,7 +1001,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3188B723-0C94-4D3B-9499-A9BB00207D84}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -891,7 +1071,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDED5571-6071-483B-91FF-46A3D4DE2E17}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -1012,7 +1192,11 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="C5" t="s">
         <v>31</v>
       </c>
@@ -1193,8 +1377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EECB696-23F9-45C5-BCAE-323A57C84042}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1203,16 +1387,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="8"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1220,7 +1404,7 @@
       <c r="A3" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1228,7 +1412,7 @@
       <c r="A4" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1236,7 +1420,7 @@
       <c r="A5" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1244,7 +1428,7 @@
       <c r="A6" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1252,7 +1436,7 @@
       <c r="A7" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1260,12 +1444,12 @@
       <c r="A8" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B9" s="1"/>
@@ -1276,4 +1460,345 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E098A59A-5D93-4B49-A446-BB06F4D5A3B7}">
+  <dimension ref="A1:C39"/>
+  <sheetViews>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.42578125" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" customWidth="1"/>
+    <col min="3" max="3" width="36.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>110</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>107</v>
+      </c>
+      <c r="B25" t="s">
+        <v>108</v>
+      </c>
+      <c r="C25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>112</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>113</v>
+      </c>
+      <c r="B29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>114</v>
+      </c>
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>116</v>
+      </c>
+      <c r="B32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>121</v>
+      </c>
+      <c r="B34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="15"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="15"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="15"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A36:C39"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A23:C23"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding starting registration feature filee
</commit_message>
<xml_diff>
--- a/Project 1/Example-RTM.xlsx
+++ b/Project 1/Example-RTM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricSuminski\Desktop\250704-JWA\Project 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD3A88E-337C-40D3-83E2-00144980C107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6898E8CF-96DA-4E32-85B5-07E0E95508A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{786AC32F-343F-4356-AB12-C2F923337BD5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{786AC32F-343F-4356-AB12-C2F923337BD5}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
@@ -499,7 +499,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -522,27 +522,21 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1001,7 +995,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3188B723-0C94-4D3B-9499-A9BB00207D84}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1377,8 +1371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EECB696-23F9-45C5-BCAE-323A57C84042}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1387,10 +1381,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="8"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -1466,8 +1460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E098A59A-5D93-4B49-A446-BB06F4D5A3B7}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1478,24 +1472,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1508,13 +1502,13 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1530,10 +1524,10 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1546,17 +1540,17 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1569,13 +1563,13 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1591,10 +1585,10 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1607,10 +1601,10 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1623,20 +1617,20 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="8" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1652,10 +1646,10 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1668,20 +1662,20 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="8" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1697,16 +1691,16 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="8" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>79</v>
+        <v>113</v>
       </c>
       <c r="B27" t="s">
         <v>32</v>
@@ -1737,10 +1731,10 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="8" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1753,10 +1747,10 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="8" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1769,26 +1763,26 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="15"/>
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1800,5 +1794,6 @@
     <mergeCell ref="A23:C23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>